<commit_message>
Add Gray Code solution and update project configuration
</commit_message>
<xml_diff>
--- a/cses.xlsx
+++ b/cses.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/myCodeBase/cses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/GitHub/cses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{950DC1E0-2D3F-EF48-9E8B-D8B30B677AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B870A94D-54AC-674E-8DF3-FB7A692B5508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="2220" windowWidth="28300" windowHeight="17440" xr2:uid="{096096B3-ED4A-BD49-8688-F427CC3ED3C9}"/>
   </bookViews>
@@ -159,7 +159,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -173,9 +173,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -539,7 +536,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -547,7 +544,6 @@
     <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="39">
@@ -579,19 +575,19 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(B:B)</f>
-        <v>1.3333333333333333</v>
+        <v>1.0833333333333333</v>
       </c>
       <c r="F2" s="2">
         <f>(400-D2)/E2</f>
-        <v>291</v>
+        <v>357.23076923076928</v>
       </c>
       <c r="G2" s="3">
         <f ca="1">TODAY()+F2</f>
-        <v>46348</v>
+        <v>46417.230769230766</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -609,16 +605,16 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>1</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f>(400-D2)/E4</f>
-        <v>388</v>
-      </c>
-      <c r="G4" s="7">
+        <v>387</v>
+      </c>
+      <c r="G4" s="6">
         <f t="shared" ref="G4:G7" ca="1" si="0">TODAY()+F4</f>
-        <v>46445</v>
+        <v>46447</v>
       </c>
       <c r="H4" s="4" t="s">
         <v>5</v>
@@ -631,18 +627,18 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>1.5</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <f>(400-D2)/E5</f>
-        <v>258.66666666666669</v>
-      </c>
-      <c r="G5" s="9">
+        <v>258</v>
+      </c>
+      <c r="G5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>46315.666666666664</v>
-      </c>
-      <c r="H5" s="5" t="s">
+        <v>46318</v>
+      </c>
+      <c r="H5" t="s">
         <v>4</v>
       </c>
     </row>
@@ -653,18 +649,18 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="9">
         <v>2</v>
       </c>
-      <c r="F6" s="10">
+      <c r="F6" s="9">
         <f>(400-D2)/E6</f>
-        <v>194</v>
-      </c>
-      <c r="G6" s="11">
+        <v>193.5</v>
+      </c>
+      <c r="G6" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>46251</v>
-      </c>
-      <c r="H6" s="5" t="s">
+        <v>46253.5</v>
+      </c>
+      <c r="H6" t="s">
         <v>6</v>
       </c>
     </row>
@@ -675,16 +671,16 @@
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>3</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <f>(400-D2)/E7</f>
-        <v>129.33333333333334</v>
-      </c>
-      <c r="G7" s="13">
+        <v>129</v>
+      </c>
+      <c r="G7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>46186.333333333336</v>
+        <v>46189</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -707,15 +703,24 @@
       <c r="A10" s="1">
         <v>46058</v>
       </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>46059</v>
       </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>46060</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8">

</xml_diff>

<commit_message>
Update binary files cses.xlsx and .DS_Store in intro directory
</commit_message>
<xml_diff>
--- a/cses.xlsx
+++ b/cses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/GitHub/cses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B870A94D-54AC-674E-8DF3-FB7A692B5508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0750921E-2014-F146-8EB6-8BB95662D538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="2220" windowWidth="28300" windowHeight="17440" xr2:uid="{096096B3-ED4A-BD49-8688-F427CC3ED3C9}"/>
+    <workbookView xWindow="1700" yWindow="2280" windowWidth="28300" windowHeight="17440" xr2:uid="{096096B3-ED4A-BD49-8688-F427CC3ED3C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -575,19 +575,19 @@
       </c>
       <c r="D2" s="2">
         <f>SUM(B:B)</f>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(B:B)</f>
-        <v>1.0833333333333333</v>
+        <v>1.1538461538461537</v>
       </c>
       <c r="F2" s="2">
         <f>(400-D2)/E2</f>
-        <v>357.23076923076928</v>
+        <v>333.66666666666669</v>
       </c>
       <c r="G2" s="3">
         <f ca="1">TODAY()+F2</f>
-        <v>46417.230769230766</v>
+        <v>46394.666666666664</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -610,14 +610,14 @@
       </c>
       <c r="F4" s="5">
         <f>(400-D2)/E4</f>
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G4" s="6">
         <f t="shared" ref="G4:G7" ca="1" si="0">TODAY()+F4</f>
-        <v>46447</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>5</v>
+        <v>46446</v>
+      </c>
+      <c r="H4" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="39">
@@ -632,14 +632,14 @@
       </c>
       <c r="F5" s="7">
         <f>(400-D2)/E5</f>
-        <v>258</v>
+        <v>256.66666666666669</v>
       </c>
       <c r="G5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>46318</v>
-      </c>
-      <c r="H5" t="s">
-        <v>4</v>
+        <v>46317.666666666664</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="39">
@@ -654,7 +654,7 @@
       </c>
       <c r="F6" s="9">
         <f>(400-D2)/E6</f>
-        <v>193.5</v>
+        <v>192.5</v>
       </c>
       <c r="G6" s="10">
         <f t="shared" ca="1" si="0"/>
@@ -676,11 +676,11 @@
       </c>
       <c r="F7" s="11">
         <f>(400-D2)/E7</f>
-        <v>129</v>
+        <v>128.33333333333334</v>
       </c>
       <c r="G7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>46189</v>
+        <v>46189.333333333336</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -726,6 +726,9 @@
     <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>46061</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:8">

</xml_diff>

<commit_message>
Add apple division problem implementation in 16appleDivision.cpp and update .gitignore
</commit_message>
<xml_diff>
--- a/cses.xlsx
+++ b/cses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harry/Desktop/GitHub/cses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0750921E-2014-F146-8EB6-8BB95662D538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4B54CFB-F188-0142-AB08-382E1904A55C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1700" yWindow="2280" windowWidth="28300" windowHeight="17440" xr2:uid="{096096B3-ED4A-BD49-8688-F427CC3ED3C9}"/>
+    <workbookView xWindow="0" yWindow="2800" windowWidth="28300" windowHeight="17440" xr2:uid="{096096B3-ED4A-BD49-8688-F427CC3ED3C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>AVG</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +63,10 @@
   </si>
   <si>
     <t>2.5h+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CF</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -159,7 +163,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -198,6 +202,9 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,11 +543,12 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
+    <col min="3" max="3" width="10.83203125" style="13"/>
     <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.6640625" bestFit="1" customWidth="1"/>
@@ -579,15 +587,15 @@
       </c>
       <c r="E2" s="2">
         <f>AVERAGE(B:B)</f>
-        <v>1.1538461538461537</v>
+        <v>0.75</v>
       </c>
       <c r="F2" s="2">
         <f>(400-D2)/E2</f>
-        <v>333.66666666666669</v>
+        <v>513.33333333333337</v>
       </c>
       <c r="G2" s="3">
         <f ca="1">TODAY()+F2</f>
-        <v>46394.666666666664</v>
+        <v>46581.333333333336</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -614,7 +622,7 @@
       </c>
       <c r="G4" s="6">
         <f t="shared" ref="G4:G7" ca="1" si="0">TODAY()+F4</f>
-        <v>46446</v>
+        <v>46453</v>
       </c>
       <c r="H4" t="s">
         <v>4</v>
@@ -636,7 +644,7 @@
       </c>
       <c r="G5" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>46317.666666666664</v>
+        <v>46324.666666666664</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>5</v>
@@ -658,7 +666,7 @@
       </c>
       <c r="G6" s="10">
         <f t="shared" ca="1" si="0"/>
-        <v>46253.5</v>
+        <v>46260.5</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
@@ -680,7 +688,7 @@
       </c>
       <c r="G7" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>46189.333333333336</v>
+        <v>46196.333333333336</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -735,93 +743,123 @@
       <c r="A14" s="1">
         <v>46062</v>
       </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>46063</v>
       </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>46064</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="1">
         <v>46065</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="1">
         <v>46066</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="1">
         <v>46067</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="1">
         <v>46068</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="1">
         <v>46069</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:3">
       <c r="A22" s="1">
         <v>46070</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:3">
       <c r="A23" s="1">
         <v>46071</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:3">
       <c r="A24" s="1">
         <v>46072</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:3">
       <c r="A25" s="1">
         <v>46073</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:3">
       <c r="A26" s="1">
         <v>46074</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:3">
       <c r="A27" s="1">
         <v>46075</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:3">
       <c r="A28" s="1">
         <v>46076</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:3">
       <c r="A29" s="1">
         <v>46077</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:3">
       <c r="A30" s="1">
         <v>46078</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:3">
       <c r="A31" s="1">
         <v>46079</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:3">
       <c r="A32" s="1">
         <v>46080</v>
       </c>

</xml_diff>